<commit_message>
Modified the start coordinates so all x values are >= 0. Negatives weren't working out so well.
</commit_message>
<xml_diff>
--- a/DataTicker3dViz/SampleData/SineAndCosine.xlsx
+++ b/DataTicker3dViz/SampleData/SineAndCosine.xlsx
@@ -386,7 +386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB979F77-9852-4678-BB3F-2A6410832CB4}">
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -403,2129 +405,2129 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>-6.5</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <f>SIN(A2)</f>
-        <v>-0.21511998808781552</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>COS(A2)</f>
-        <v>0.97658762572802349</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+0.1</f>
-        <v>-6.4</v>
+        <v>0.1</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" si="0">SIN(A3)</f>
-        <v>-0.11654920485049364</v>
+        <v>9.9833416646828155E-2</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" si="1">COS(A3)</f>
-        <v>0.99318491875819259</v>
+        <v>0.99500416527802582</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="2">A3+0.1</f>
-        <v>-6.3000000000000007</v>
+        <v>0.2</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>-1.6813900484350601E-2</v>
+        <v>0.19866933079506122</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>0.9998586363834151</v>
+        <v>0.98006657784124163</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="2"/>
-        <v>-6.2000000000000011</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>8.3089402817495522E-2</v>
+        <v>0.2955202066613396</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>0.99654209702321761</v>
+        <v>0.95533648912560598</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="2"/>
-        <v>-6.1000000000000014</v>
+        <v>0.4</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>0.18216250427209416</v>
+        <v>0.38941834230865052</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>0.98326843844258482</v>
+        <v>0.9210609940028851</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="2"/>
-        <v>-6.0000000000000018</v>
+        <v>0.5</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0.27941549819892419</v>
+        <v>0.47942553860420301</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0.96017028665036652</v>
+        <v>0.87758256189037276</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="2"/>
-        <v>-5.9000000000000021</v>
+        <v>0.6</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.37387666483023441</v>
+        <v>0.56464247339503537</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>0.92747843074403657</v>
+        <v>0.82533561490967833</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="2"/>
-        <v>-5.8000000000000025</v>
+        <v>0.7</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0.46460217941375503</v>
+        <v>0.64421768723769102</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0.88551951694132014</v>
+        <v>0.7648421872844885</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="2"/>
-        <v>-5.7000000000000028</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.55068554259763536</v>
+        <v>0.71735609089952268</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>0.83471278483916123</v>
+        <v>0.6967067093471655</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="2"/>
-        <v>-5.6000000000000032</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>0.63126663787231885</v>
+        <v>0.7833269096274833</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>0.77556587851025183</v>
+        <v>0.6216099682706645</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="2"/>
-        <v>-5.5000000000000036</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0.70554032557038937</v>
+        <v>0.84147098480789639</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>0.70866977429126254</v>
+        <v>0.54030230586813977</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="2"/>
-        <v>-5.4000000000000039</v>
+        <v>1.0999999999999999</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>0.77276448755598492</v>
+        <v>0.89120736006143531</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>0.63469287594263735</v>
+        <v>0.45359612142557748</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="2"/>
-        <v>-5.3000000000000043</v>
+        <v>1.2</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>0.83226744222389881</v>
+        <v>0.93203908596722629</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>0.55437433617916443</v>
+        <v>0.36235775447667362</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="2"/>
-        <v>-5.2000000000000046</v>
+        <v>1.3</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>0.88345465572015114</v>
+        <v>0.96355818541719296</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0.46851667130038105</v>
+        <v>0.26749882862458735</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="2"/>
-        <v>-5.100000000000005</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>0.92581468232773045</v>
+        <v>0.98544972998846025</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>0.37797774271298518</v>
+        <v>0.16996714290024081</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="2"/>
-        <v>-5.0000000000000053</v>
+        <v>1.5000000000000002</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>0.95892427466313701</v>
+        <v>0.99749498660405445</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>0.28366218546323135</v>
+        <v>7.0737201667702684E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="2"/>
-        <v>-4.9000000000000057</v>
+        <v>1.6000000000000003</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>0.98245261262433148</v>
+        <v>0.99957360304150511</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0.18651236942258098</v>
+        <v>-2.9199522301289037E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="2"/>
-        <v>-4.800000000000006</v>
+        <v>1.7000000000000004</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>0.99616460883584013</v>
+        <v>0.99166481045246857</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>8.7498983439452588E-2</v>
+        <v>-0.12884449429552508</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="2"/>
-        <v>-4.7000000000000064</v>
+        <v>1.8000000000000005</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>0.99992325756410094</v>
+        <v>0.97384763087819504</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>-1.2388663462884343E-2</v>
+        <v>-0.22720209469308753</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="2"/>
-        <v>-4.6000000000000068</v>
+        <v>1.9000000000000006</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>0.99369100363346519</v>
+        <v>0.94630008768741425</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>-0.11215252693504781</v>
+        <v>-0.32328956686350396</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="2"/>
-        <v>-4.5000000000000071</v>
+        <v>2.0000000000000004</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>0.97753011766509856</v>
+        <v>0.90929742682568149</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>-0.21079579943077276</v>
+        <v>-0.4161468365471428</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="2"/>
-        <v>-4.4000000000000075</v>
+        <v>2.1000000000000005</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>0.95160207388951823</v>
+        <v>0.86320936664887349</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>-0.30733286997841258</v>
+        <v>-0.5048461045998579</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="2"/>
-        <v>-4.3000000000000078</v>
+        <v>2.2000000000000006</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>0.91616593674945812</v>
+        <v>0.80849640381958987</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>-0.40079917207996812</v>
+        <v>-0.58850111725534626</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="2"/>
-        <v>-4.2000000000000082</v>
+        <v>2.3000000000000007</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>0.87157577241359208</v>
+        <v>0.7457052121767197</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>-0.49026082134069243</v>
+        <v>-0.66627602127982477</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="2"/>
-        <v>-4.1000000000000085</v>
+        <v>2.4000000000000008</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>0.81827711106441536</v>
+        <v>0.67546318055115029</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>-0.57482394653326196</v>
+        <v>-0.737393715541246</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="2"/>
-        <v>-4.0000000000000089</v>
+        <v>2.5000000000000009</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>0.75680249530793409</v>
+        <v>0.59847214410395577</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>-0.65364362086360517</v>
+        <v>-0.80114361554693425</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="2"/>
-        <v>-3.9000000000000088</v>
+        <v>2.600000000000001</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>0.68776615918398021</v>
+        <v>0.51550137182146338</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>-0.7259323042001341</v>
+        <v>-0.85688875336894776</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="2"/>
-        <v>-3.8000000000000087</v>
+        <v>2.7000000000000011</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>0.61185789094272591</v>
+        <v>0.42737988023382895</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>-0.7909677119144114</v>
+        <v>-0.90407214201706165</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="2"/>
-        <v>-3.7000000000000086</v>
+        <v>2.8000000000000012</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>0.52983614090850051</v>
+        <v>0.33498815015590383</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>-0.8481000317104036</v>
+        <v>-0.94222234066865851</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="2"/>
-        <v>-3.6000000000000085</v>
+        <v>2.9000000000000012</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>0.44252044329486001</v>
+        <v>0.23924932921398112</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>-0.89675841633414322</v>
+        <v>-0.97095816514959077</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="2"/>
-        <v>-3.5000000000000084</v>
+        <v>3.0000000000000013</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>0.35078322768962777</v>
+        <v>0.14112000805986591</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>-0.93645668729079334</v>
+        <v>-0.98999249660044564</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="2"/>
-        <v>-3.4000000000000083</v>
+        <v>3.1000000000000014</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>0.25554110202683938</v>
+        <v>4.1580662433289159E-2</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>-0.96679819257945887</v>
+        <v>-0.99913515027327948</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="2"/>
-        <v>-3.3000000000000083</v>
+        <v>3.2000000000000015</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>0.15774569414325654</v>
+        <v>-5.8374143427581418E-2</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>-0.98747976990886355</v>
+        <v>-0.99829477579475301</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="2"/>
-        <v>-3.2000000000000082</v>
+        <v>3.3000000000000016</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>5.8374143427588066E-2</v>
+        <v>-0.15774569414324996</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>-0.99829477579475256</v>
+        <v>-0.98747976990886466</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="2"/>
-        <v>-3.1000000000000081</v>
+        <v>3.4000000000000017</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>-4.1580662433282504E-2</v>
+        <v>-0.25554110202683294</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>-0.99913515027327982</v>
+        <v>-0.96679819257946054</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="2"/>
-        <v>-3.000000000000008</v>
+        <v>3.5000000000000018</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>-0.1411200080598593</v>
+        <v>-0.3507832276896215</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>-0.98999249660044664</v>
+        <v>-0.93645668729079568</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="2"/>
-        <v>-2.9000000000000079</v>
+        <v>3.6000000000000019</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>-0.23924932921397465</v>
+        <v>-0.44252044329485407</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>-0.97095816514959243</v>
+        <v>-0.89675841633414621</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="2"/>
-        <v>-2.8000000000000078</v>
+        <v>3.700000000000002</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>-0.33498815015589756</v>
+        <v>-0.52983614090849485</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>-0.94222234066866073</v>
+        <v>-0.84810003171040715</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="2"/>
-        <v>-2.7000000000000077</v>
+        <v>3.800000000000002</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>-0.42737988023382295</v>
+        <v>-0.61185789094272069</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>-0.90407214201706443</v>
+        <v>-0.79096771191441551</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="2"/>
-        <v>-2.6000000000000076</v>
+        <v>3.9000000000000021</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>-0.51550137182145772</v>
+        <v>-0.68776615918397532</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>-0.85688875336895121</v>
+        <v>-0.72593230420013866</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="2"/>
-        <v>-2.5000000000000075</v>
+        <v>4.0000000000000018</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>-0.59847214410395044</v>
+        <v>-0.75680249530792942</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>-0.80114361554693825</v>
+        <v>-0.65364362086361061</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="2"/>
-        <v>-2.4000000000000075</v>
+        <v>4.1000000000000014</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>-0.6754631805511454</v>
+        <v>-0.81827711106441137</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>-0.73739371554125055</v>
+        <v>-0.57482394653326774</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="2"/>
-        <v>-2.3000000000000074</v>
+        <v>4.2000000000000011</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>-0.74570521217671526</v>
+        <v>-0.87157577241358863</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>-0.66627602127982966</v>
+        <v>-0.49026082134069865</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="2"/>
-        <v>-2.2000000000000073</v>
+        <v>4.3000000000000007</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>-0.80849640381958587</v>
+        <v>-0.91616593674945523</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>-0.58850111725535159</v>
+        <v>-0.40079917207997462</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="2"/>
-        <v>-2.1000000000000072</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>-0.86320936664887016</v>
+        <v>-0.95160207388951601</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>-0.50484610459986368</v>
+        <v>-0.30733286997841935</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="2"/>
-        <v>-2.0000000000000071</v>
+        <v>4.5</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>-0.90929742682567871</v>
+        <v>-0.97753011766509701</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>-0.41614683654714885</v>
+        <v>-0.2107957994307797</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="2"/>
-        <v>-1.900000000000007</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>-0.94630008768741225</v>
+        <v>-0.99369100363346441</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>-0.32328956686351007</v>
+        <v>-0.11215252693505487</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="2"/>
-        <v>-1.8000000000000069</v>
+        <v>4.6999999999999993</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>-0.97384763087819359</v>
+        <v>-0.99992325756410083</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>-0.2272020946930938</v>
+        <v>-1.2388663462891449E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="2"/>
-        <v>-1.7000000000000068</v>
+        <v>4.7999999999999989</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>-0.99166481045246768</v>
+        <v>-0.99616460883584079</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>-0.12884449429553146</v>
+        <v>8.749898343944551E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="2"/>
-        <v>-1.6000000000000068</v>
+        <v>4.8999999999999986</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>-0.999573603041505</v>
+        <v>-0.98245261262433281</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>-2.9199522301295473E-2</v>
+        <v>0.18651236942257401</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="2"/>
-        <v>-1.5000000000000067</v>
+        <v>4.9999999999999982</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>-0.99749498660405489</v>
+        <v>-0.95892427466313901</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>7.0737201667696259E-2</v>
+        <v>0.28366218546322458</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="2"/>
-        <v>-1.4000000000000066</v>
+        <v>5.0999999999999979</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>-0.98544972998846125</v>
+        <v>-0.92581468232773312</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>0.16996714290023446</v>
+        <v>0.37797774271297857</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="2"/>
-        <v>-1.3000000000000065</v>
+        <v>5.1999999999999975</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>-0.96355818541719473</v>
+        <v>-0.88345465572015447</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>0.26749882862458119</v>
+        <v>0.46851667130037478</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="2"/>
-        <v>-1.2000000000000064</v>
+        <v>5.2999999999999972</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>-0.93203908596722862</v>
+        <v>-0.8322674422239027</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>0.36235775447666763</v>
+        <v>0.55437433617915854</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="2"/>
-        <v>-1.1000000000000063</v>
+        <v>5.3999999999999968</v>
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>-0.89120736006143819</v>
+        <v>-0.77276448755598937</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>0.45359612142557176</v>
+        <v>0.63469287594263191</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="2"/>
-        <v>-1.0000000000000062</v>
+        <v>5.4999999999999964</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>-0.84147098480789984</v>
+        <v>-0.70554032557039448</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>0.54030230586813444</v>
+        <v>0.70866977429125755</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="2"/>
-        <v>-0.90000000000000624</v>
+        <v>5.5999999999999961</v>
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>-0.7833269096274873</v>
+        <v>-0.63126663787232429</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>0.62160996827065962</v>
+        <v>0.77556587851024728</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="2"/>
-        <v>-0.80000000000000626</v>
+        <v>5.6999999999999957</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>-0.71735609089952712</v>
+        <v>-0.55068554259764135</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>0.69670670934716095</v>
+        <v>0.83471278483915734</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="2"/>
-        <v>-0.70000000000000628</v>
+        <v>5.7999999999999954</v>
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>-0.6442176872376959</v>
+        <v>-0.46460217941376131</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>0.76484218728448439</v>
+        <v>0.88551951694131681</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="2"/>
-        <v>-0.60000000000000631</v>
+        <v>5.899999999999995</v>
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>-0.56464247339504059</v>
+        <v>-0.37387666483024096</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
-        <v>0.82533561490967478</v>
+        <v>0.92747843074403391</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="2"/>
-        <v>-0.50000000000000633</v>
+        <v>5.9999999999999947</v>
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>-0.47942553860420856</v>
+        <v>-0.27941549819893097</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
-        <v>0.87758256189036965</v>
+        <v>0.96017028665036452</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="2"/>
-        <v>-0.40000000000000635</v>
+        <v>6.0999999999999943</v>
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>-0.38941834230865635</v>
+        <v>-0.18216250427210112</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
-        <v>0.92106099400288266</v>
+        <v>0.9832684384425836</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="2"/>
-        <v>-0.30000000000000637</v>
+        <v>6.199999999999994</v>
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>-0.29552020666134565</v>
+        <v>-8.30894028175026E-2</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
-        <v>0.95533648912560409</v>
+        <v>0.99654209702321694</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="2"/>
-        <v>-0.20000000000000637</v>
+        <v>6.2999999999999936</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>-0.19866933079506746</v>
+        <v>1.6813900484343496E-2</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
-        <v>0.98006657784124041</v>
+        <v>0.99985863638341521</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="2"/>
-        <v>-0.10000000000000636</v>
+        <v>6.3999999999999932</v>
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>-9.9833416646834483E-2</v>
+        <v>0.11654920485048659</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
-        <v>0.99500416527802515</v>
+        <v>0.99318491875819348</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" si="2"/>
-        <v>-6.3560268159790212E-15</v>
+        <v>6.4999999999999929</v>
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B130" si="3">SIN(A67)</f>
-        <v>-6.3560268159790212E-15</v>
+        <v>0.21511998808780858</v>
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C130" si="4">COS(A67)</f>
-        <v>1</v>
+        <v>0.97658762572802504</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" ref="A68:A131" si="5">A67+0.1</f>
-        <v>9.999999999999365E-2</v>
+        <v>6.5999999999999925</v>
       </c>
       <c r="B68">
         <f t="shared" si="3"/>
-        <v>9.983341664682184E-2</v>
+        <v>0.31154136351337108</v>
       </c>
       <c r="C68">
         <f t="shared" si="4"/>
-        <v>0.99500416527802638</v>
+        <v>0.95023259195853182</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="5"/>
-        <v>0.19999999999999366</v>
+        <v>6.6999999999999922</v>
       </c>
       <c r="B69">
         <f t="shared" si="3"/>
-        <v>0.198669330795055</v>
+        <v>0.40484992061659103</v>
       </c>
       <c r="C69">
         <f t="shared" si="4"/>
-        <v>0.98006657784124285</v>
+        <v>0.91438314823532263</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="5"/>
-        <v>0.29999999999999366</v>
+        <v>6.7999999999999918</v>
       </c>
       <c r="B70">
         <f t="shared" si="3"/>
-        <v>0.2955202066613335</v>
+        <v>0.49411335113860122</v>
       </c>
       <c r="C70">
         <f t="shared" si="4"/>
-        <v>0.95533648912560787</v>
+        <v>0.86939749034982916</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="5"/>
-        <v>0.39999999999999369</v>
+        <v>6.8999999999999915</v>
       </c>
       <c r="B71">
         <f t="shared" si="3"/>
-        <v>0.38941834230864469</v>
+        <v>0.57843976438819289</v>
       </c>
       <c r="C71">
         <f t="shared" si="4"/>
-        <v>0.92106099400288755</v>
+        <v>0.81572510012536203</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="5"/>
-        <v>0.49999999999999367</v>
+        <v>6.9999999999999911</v>
       </c>
       <c r="B72">
         <f t="shared" si="3"/>
-        <v>0.47942553860419745</v>
+        <v>0.6569865987187824</v>
       </c>
       <c r="C72">
         <f t="shared" si="4"/>
-        <v>0.87758256189037576</v>
+        <v>0.75390225434331049</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="5"/>
-        <v>0.59999999999999365</v>
+        <v>7.0999999999999908</v>
       </c>
       <c r="B73">
         <f t="shared" si="3"/>
-        <v>0.56464247339503015</v>
+        <v>0.72896904012586983</v>
       </c>
       <c r="C73">
         <f t="shared" si="4"/>
-        <v>0.82533561490968188</v>
+        <v>0.68454666644281303</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="5"/>
-        <v>0.69999999999999363</v>
+        <v>7.1999999999999904</v>
       </c>
       <c r="B74">
         <f t="shared" si="3"/>
-        <v>0.64421768723768613</v>
+        <v>0.79366786384914723</v>
       </c>
       <c r="C74">
         <f t="shared" si="4"/>
-        <v>0.76484218728449249</v>
+        <v>0.60835131453226232</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="5"/>
-        <v>0.79999999999999361</v>
+        <v>7.2999999999999901</v>
       </c>
       <c r="B75">
         <f t="shared" si="3"/>
-        <v>0.71735609089951835</v>
+        <v>0.85043662062855929</v>
       </c>
       <c r="C75">
         <f t="shared" si="4"/>
-        <v>0.69670670934717005</v>
+        <v>0.52607751738111364</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="5"/>
-        <v>0.89999999999999358</v>
+        <v>7.3999999999999897</v>
       </c>
       <c r="B76">
         <f t="shared" si="3"/>
-        <v>0.78332690962747942</v>
+        <v>0.89870809581162225</v>
       </c>
       <c r="C76">
         <f t="shared" si="4"/>
-        <v>0.6216099682706695</v>
+        <v>0.4385473275743999</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="5"/>
-        <v>0.99999999999999356</v>
+        <v>7.4999999999999893</v>
       </c>
       <c r="B77">
         <f t="shared" si="3"/>
-        <v>0.84147098480789306</v>
+        <v>0.93799997677473512</v>
       </c>
       <c r="C77">
         <f t="shared" si="4"/>
-        <v>0.54030230586814509</v>
+        <v>0.34663531783503582</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="5"/>
-        <v>1.0999999999999936</v>
+        <v>7.599999999999989</v>
       </c>
       <c r="B78">
         <f t="shared" si="3"/>
-        <v>0.89120736006143242</v>
+        <v>0.96791967203148366</v>
       </c>
       <c r="C78">
         <f t="shared" si="4"/>
-        <v>0.45359612142558303</v>
+        <v>0.25125984258226602</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="5"/>
-        <v>1.1999999999999937</v>
+        <v>7.6999999999999886</v>
       </c>
       <c r="B79">
         <f t="shared" si="3"/>
-        <v>0.93203908596722407</v>
+        <v>0.98816823387699859</v>
       </c>
       <c r="C79">
         <f t="shared" si="4"/>
-        <v>0.36235775447667939</v>
+        <v>0.15337386203787576</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="5"/>
-        <v>1.2999999999999938</v>
+        <v>7.7999999999999883</v>
       </c>
       <c r="B80">
         <f t="shared" si="3"/>
-        <v>0.96355818541719129</v>
+        <v>0.99854334537460432</v>
       </c>
       <c r="C80">
         <f t="shared" si="4"/>
-        <v>0.26749882862459334</v>
+        <v>5.3955420562661283E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="5"/>
-        <v>1.3999999999999939</v>
+        <v>7.8999999999999879</v>
       </c>
       <c r="B81">
         <f t="shared" si="3"/>
-        <v>0.98544972998845914</v>
+        <v>0.99894134183977257</v>
       </c>
       <c r="C81">
         <f t="shared" si="4"/>
-        <v>0.16996714290024692</v>
+        <v>-4.6002125639524528E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="5"/>
-        <v>1.499999999999994</v>
+        <v>7.9999999999999876</v>
       </c>
       <c r="B82">
         <f t="shared" si="3"/>
-        <v>0.997494986604054</v>
+        <v>0.98935824662338356</v>
       </c>
       <c r="C82">
         <f t="shared" si="4"/>
-        <v>7.0737201667708888E-2</v>
+        <v>-0.14550003380860121</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="5"/>
-        <v>1.5999999999999941</v>
+        <v>8.0999999999999872</v>
       </c>
       <c r="B83">
         <f t="shared" si="3"/>
-        <v>0.99957360304150533</v>
+        <v>0.96988981084508941</v>
       </c>
       <c r="C83">
         <f t="shared" si="4"/>
-        <v>-2.9199522301282824E-2</v>
+        <v>-0.24354415373577906</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="5"/>
-        <v>1.6999999999999942</v>
+        <v>8.1999999999999869</v>
       </c>
       <c r="B84">
         <f t="shared" si="3"/>
-        <v>0.99166481045246935</v>
+        <v>0.94073055667977734</v>
       </c>
       <c r="C84">
         <f t="shared" si="4"/>
-        <v>-0.12884449429551892</v>
+        <v>-0.33915486098382286</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="5"/>
-        <v>1.7999999999999943</v>
+        <v>8.2999999999999865</v>
       </c>
       <c r="B85">
         <f t="shared" si="3"/>
-        <v>0.97384763087819648</v>
+        <v>0.9021718337562995</v>
       </c>
       <c r="C85">
         <f t="shared" si="4"/>
-        <v>-0.22720209469308147</v>
+        <v>-0.43137684497060802</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="5"/>
-        <v>1.8999999999999944</v>
+        <v>8.3999999999999861</v>
       </c>
       <c r="B86">
         <f t="shared" si="3"/>
-        <v>0.94630008768741636</v>
+        <v>0.85459890808828787</v>
       </c>
       <c r="C86">
         <f t="shared" si="4"/>
-        <v>-0.32328956686349808</v>
+        <v>-0.51928865411667346</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="5"/>
-        <v>1.9999999999999944</v>
+        <v>8.4999999999999858</v>
       </c>
       <c r="B87">
         <f t="shared" si="3"/>
-        <v>0.90929742682568404</v>
+        <v>0.79848711262349881</v>
       </c>
       <c r="C87">
         <f t="shared" si="4"/>
-        <v>-0.41614683654713736</v>
+        <v>-0.60201190268481231</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="5"/>
-        <v>2.0999999999999943</v>
+        <v>8.5999999999999854</v>
       </c>
       <c r="B88">
         <f t="shared" si="3"/>
-        <v>0.8632093666488766</v>
+        <v>0.73439709787412299</v>
       </c>
       <c r="C88">
         <f t="shared" si="4"/>
-        <v>-0.50484610459985257</v>
+        <v>-0.67872004732000202</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="5"/>
-        <v>2.1999999999999944</v>
+        <v>8.6999999999999851</v>
       </c>
       <c r="B89">
         <f t="shared" si="3"/>
-        <v>0.80849640381959342</v>
+        <v>0.66296923008219399</v>
       </c>
       <c r="C89">
         <f t="shared" si="4"/>
-        <v>-0.58850111725534116</v>
+        <v>-0.74864664559738925</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="5"/>
-        <v>2.2999999999999945</v>
+        <v>8.7999999999999847</v>
       </c>
       <c r="B90">
         <f t="shared" si="3"/>
-        <v>0.74570521217672381</v>
+        <v>0.58491719289177468</v>
       </c>
       <c r="C90">
         <f t="shared" si="4"/>
-        <v>-0.66627602127982011</v>
+        <v>-0.81109301406164658</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="5"/>
-        <v>2.3999999999999946</v>
+        <v>8.8999999999999844</v>
       </c>
       <c r="B91">
         <f t="shared" si="3"/>
-        <v>0.67546318055115495</v>
+        <v>0.50102085645789851</v>
       </c>
       <c r="C91">
         <f t="shared" si="4"/>
-        <v>-0.73739371554124189</v>
+        <v>-0.86543520924110418</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="5"/>
-        <v>2.4999999999999947</v>
+        <v>8.999999999999984</v>
       </c>
       <c r="B92">
         <f t="shared" si="3"/>
-        <v>0.59847214410396077</v>
+        <v>0.41211848524177114</v>
       </c>
       <c r="C92">
         <f t="shared" si="4"/>
-        <v>-0.80114361554693048</v>
+        <v>-0.91113026188467039</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="5"/>
-        <v>2.5999999999999948</v>
+        <v>9.0999999999999837</v>
       </c>
       <c r="B93">
         <f t="shared" si="3"/>
-        <v>0.51550137182146871</v>
+        <v>0.31909836234936728</v>
       </c>
       <c r="C93">
         <f t="shared" si="4"/>
-        <v>-0.85688875336894454</v>
+        <v>-0.94772160213110679</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="5"/>
-        <v>2.6999999999999948</v>
+        <v>9.1999999999999833</v>
       </c>
       <c r="B94">
         <f t="shared" si="3"/>
-        <v>0.42737988023383461</v>
+        <v>0.22288991410026324</v>
       </c>
       <c r="C94">
         <f t="shared" si="4"/>
-        <v>-0.90407214201705899</v>
+        <v>-0.97484362140416003</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="5"/>
-        <v>2.7999999999999949</v>
+        <v>9.2999999999999829</v>
       </c>
       <c r="B95">
         <f t="shared" si="3"/>
-        <v>0.33498815015590971</v>
+        <v>0.12445442350707933</v>
       </c>
       <c r="C95">
         <f t="shared" si="4"/>
-        <v>-0.94222234066865651</v>
+        <v>-0.99222532545260134</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <f t="shared" si="5"/>
-        <v>2.899999999999995</v>
+        <v>9.3999999999999826</v>
       </c>
       <c r="B96">
         <f t="shared" si="3"/>
-        <v>0.23924932921398714</v>
+        <v>2.4775425453375525E-2</v>
       </c>
       <c r="C96">
         <f t="shared" si="4"/>
-        <v>-0.97095816514958933</v>
+        <v>-0.99969304203520604</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="5"/>
-        <v>2.9999999999999951</v>
+        <v>9.4999999999999822</v>
       </c>
       <c r="B97">
         <f t="shared" si="3"/>
-        <v>0.14112000805987207</v>
+        <v>-7.5151120461791593E-2</v>
       </c>
       <c r="C97">
         <f t="shared" si="4"/>
-        <v>-0.98999249660044475</v>
+        <v>-0.99717215619637978</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="5"/>
-        <v>3.0999999999999952</v>
+        <v>9.5999999999999819</v>
       </c>
       <c r="B98">
         <f t="shared" si="3"/>
-        <v>4.1580662433295369E-2</v>
+        <v>-0.17432678122296213</v>
       </c>
       <c r="C98">
         <f t="shared" si="4"/>
-        <v>-0.99913515027327926</v>
+        <v>-0.9846878557941301</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <f t="shared" si="5"/>
-        <v>3.1999999999999953</v>
+        <v>9.6999999999999815</v>
       </c>
       <c r="B99">
         <f t="shared" si="3"/>
-        <v>-5.8374143427575208E-2</v>
+        <v>-0.27176062641092535</v>
       </c>
       <c r="C99">
         <f t="shared" si="4"/>
-        <v>-0.99829477579475334</v>
+        <v>-0.96236487983131502</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="5"/>
-        <v>3.2999999999999954</v>
+        <v>9.7999999999999812</v>
       </c>
       <c r="B100">
         <f t="shared" si="3"/>
-        <v>-0.15774569414324383</v>
+        <v>-0.36647912925191023</v>
       </c>
       <c r="C100">
         <f t="shared" si="4"/>
-        <v>-0.98747976990886566</v>
+        <v>-0.93042627210476037</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <f t="shared" si="5"/>
-        <v>3.3999999999999955</v>
+        <v>9.8999999999999808</v>
       </c>
       <c r="B101">
         <f t="shared" si="3"/>
-        <v>-0.25554110202682695</v>
+        <v>-0.45753589377530396</v>
       </c>
       <c r="C101">
         <f t="shared" si="4"/>
-        <v>-0.9667981925794622</v>
+        <v>-0.88919115262536985</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <f t="shared" si="5"/>
-        <v>3.4999999999999956</v>
+        <v>9.9999999999999805</v>
       </c>
       <c r="B102">
         <f t="shared" si="3"/>
-        <v>-0.35078322768961567</v>
+        <v>-0.54402111088935345</v>
       </c>
       <c r="C102">
         <f t="shared" si="4"/>
-        <v>-0.9364566872907979</v>
+        <v>-0.8390715290764631</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <f t="shared" si="5"/>
-        <v>3.5999999999999956</v>
+        <v>10.09999999999998</v>
       </c>
       <c r="B103">
         <f t="shared" si="3"/>
-        <v>-0.44252044329484846</v>
+        <v>-0.62507064889286679</v>
       </c>
       <c r="C103">
         <f t="shared" si="4"/>
-        <v>-0.89675841633414888</v>
+        <v>-0.78056818016919594</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <f t="shared" si="5"/>
-        <v>3.6999999999999957</v>
+        <v>10.19999999999998</v>
       </c>
       <c r="B104">
         <f t="shared" si="3"/>
-        <v>-0.52983614090848963</v>
+        <v>-0.69987468759352844</v>
       </c>
       <c r="C104">
         <f t="shared" si="4"/>
-        <v>-0.84810003171041037</v>
+        <v>-0.71426565202721393</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <f t="shared" si="5"/>
-        <v>3.7999999999999958</v>
+        <v>10.299999999999979</v>
       </c>
       <c r="B105">
         <f t="shared" si="3"/>
-        <v>-0.61185789094271581</v>
+        <v>-0.76768580976356882</v>
       </c>
       <c r="C105">
         <f t="shared" si="4"/>
-        <v>-0.79096771191441928</v>
+        <v>-0.64082641759500969</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <f t="shared" si="5"/>
-        <v>3.8999999999999959</v>
+        <v>10.399999999999979</v>
       </c>
       <c r="B106">
         <f t="shared" si="3"/>
-        <v>-0.68776615918397088</v>
+        <v>-0.82782646908564173</v>
       </c>
       <c r="C106">
         <f t="shared" si="4"/>
-        <v>-0.72593230420014299</v>
+        <v>-0.56098425742724645</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <f t="shared" si="5"/>
-        <v>3.999999999999996</v>
+        <v>10.499999999999979</v>
       </c>
       <c r="B107">
         <f t="shared" si="3"/>
-        <v>-0.75680249530792565</v>
+        <v>-0.87969575997165994</v>
       </c>
       <c r="C107">
         <f t="shared" si="4"/>
-        <v>-0.65364362086361494</v>
+        <v>-0.47553692799601127</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <f t="shared" si="5"/>
-        <v>4.0999999999999961</v>
+        <v>10.599999999999978</v>
       </c>
       <c r="B108">
         <f t="shared" si="3"/>
-        <v>-0.81827711106440826</v>
+        <v>-0.92277542161279846</v>
       </c>
       <c r="C108">
         <f t="shared" si="4"/>
-        <v>-0.57482394653327207</v>
+        <v>-0.38533819077184933</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <f t="shared" si="5"/>
-        <v>4.1999999999999957</v>
+        <v>10.699999999999978</v>
       </c>
       <c r="B109">
         <f t="shared" si="3"/>
-        <v>-0.87157577241358597</v>
+        <v>-0.95663501627018166</v>
       </c>
       <c r="C109">
         <f t="shared" si="4"/>
-        <v>-0.49026082134070331</v>
+        <v>-0.29128928172136592</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
         <f t="shared" si="5"/>
-        <v>4.2999999999999954</v>
+        <v>10.799999999999978</v>
       </c>
       <c r="B110">
         <f t="shared" si="3"/>
-        <v>-0.91616593674945312</v>
+        <v>-0.980936230066487</v>
       </c>
       <c r="C110">
         <f t="shared" si="4"/>
-        <v>-0.4007991720799795</v>
+        <v>-0.19432990645535744</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <f t="shared" si="5"/>
-        <v>4.399999999999995</v>
+        <v>10.899999999999977</v>
       </c>
       <c r="B111">
         <f t="shared" si="3"/>
-        <v>-0.95160207388951445</v>
+        <v>-0.9954362533063752</v>
       </c>
       <c r="C111">
         <f t="shared" si="4"/>
-        <v>-0.30733286997842441</v>
+        <v>-9.5428851000973647E-2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
         <f t="shared" si="5"/>
-        <v>4.4999999999999947</v>
+        <v>10.999999999999977</v>
       </c>
       <c r="B112">
         <f t="shared" si="3"/>
-        <v>-0.9775301176650959</v>
+        <v>-0.99999020655070359</v>
       </c>
       <c r="C112">
         <f t="shared" si="4"/>
-        <v>-0.21079579943078491</v>
+        <v>4.4256979880276928E-3</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <f t="shared" si="5"/>
-        <v>4.5999999999999943</v>
+        <v>11.099999999999977</v>
       </c>
       <c r="B113">
         <f t="shared" si="3"/>
-        <v>-0.99369100363346385</v>
+        <v>-0.99455258820399162</v>
       </c>
       <c r="C113">
         <f t="shared" si="4"/>
-        <v>-0.11215252693506017</v>
+        <v>0.10423602686567392</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
         <f t="shared" si="5"/>
-        <v>4.699999999999994</v>
+        <v>11.199999999999976</v>
       </c>
       <c r="B114">
         <f t="shared" si="3"/>
-        <v>-0.99992325756410083</v>
+        <v>-0.97917772915132206</v>
       </c>
       <c r="C114">
         <f t="shared" si="4"/>
-        <v>-1.2388663462896776E-2</v>
+        <v>0.20300486381872779</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <f t="shared" si="5"/>
-        <v>4.7999999999999936</v>
+        <v>11.299999999999976</v>
       </c>
       <c r="B115">
         <f t="shared" si="3"/>
-        <v>-0.99616460883584124</v>
+        <v>-0.95401924990209641</v>
       </c>
       <c r="C115">
         <f t="shared" si="4"/>
-        <v>8.7498983439440195E-2</v>
+        <v>0.29974534327699121</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
         <f t="shared" si="5"/>
-        <v>4.8999999999999932</v>
+        <v>11.399999999999975</v>
       </c>
       <c r="B116">
         <f t="shared" si="3"/>
-        <v>-0.98245261262433381</v>
+        <v>-0.91932852566468548</v>
       </c>
       <c r="C116">
         <f t="shared" si="4"/>
-        <v>0.18651236942256877</v>
+        <v>0.39349086634786806</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
         <f t="shared" si="5"/>
-        <v>4.9999999999999929</v>
+        <v>11.499999999999975</v>
       </c>
       <c r="B117">
         <f t="shared" si="3"/>
-        <v>-0.95892427466314045</v>
+        <v>-0.8754521746884405</v>
       </c>
       <c r="C117">
         <f t="shared" si="4"/>
-        <v>0.28366218546321947</v>
+        <v>0.48330475875298412</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
         <f t="shared" si="5"/>
-        <v>5.0999999999999925</v>
+        <v>11.599999999999975</v>
       </c>
       <c r="B118">
         <f t="shared" si="3"/>
-        <v>-0.92581468232773512</v>
+        <v>-0.82282859496872296</v>
       </c>
       <c r="C118">
         <f t="shared" si="4"/>
-        <v>0.37797774271297363</v>
+        <v>0.56828962976795316</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
         <f t="shared" si="5"/>
-        <v>5.1999999999999922</v>
+        <v>11.699999999999974</v>
       </c>
       <c r="B119">
         <f t="shared" si="3"/>
-        <v>-0.88345465572015691</v>
+        <v>-0.76198358391904941</v>
       </c>
       <c r="C119">
         <f t="shared" si="4"/>
-        <v>0.46851667130037006</v>
+        <v>0.64759633865385702</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
         <f t="shared" si="5"/>
-        <v>5.2999999999999918</v>
+        <v>11.799999999999974</v>
       </c>
       <c r="B120">
         <f t="shared" si="3"/>
-        <v>-0.8322674422239057</v>
+        <v>-0.69352508477714159</v>
       </c>
       <c r="C120">
         <f t="shared" si="4"/>
-        <v>0.5543743361791541</v>
+        <v>0.72043247899082019</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
         <f t="shared" si="5"/>
-        <v>5.3999999999999915</v>
+        <v>11.899999999999974</v>
       </c>
       <c r="B121">
         <f t="shared" si="3"/>
-        <v>-0.77276448755599281</v>
+        <v>-0.61813711223705425</v>
       </c>
       <c r="C121">
         <f t="shared" si="4"/>
-        <v>0.6346928759426278</v>
+        <v>0.78607029614102286</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122">
         <f t="shared" si="5"/>
-        <v>5.4999999999999911</v>
+        <v>11.999999999999973</v>
       </c>
       <c r="B122">
         <f t="shared" si="3"/>
-        <v>-0.70554032557039825</v>
+        <v>-0.53657291800045748</v>
       </c>
       <c r="C122">
         <f t="shared" si="4"/>
-        <v>0.70866977429125377</v>
+        <v>0.84385395873247782</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
         <f t="shared" si="5"/>
-        <v>5.5999999999999908</v>
+        <v>12.099999999999973</v>
       </c>
       <c r="B123">
         <f t="shared" si="3"/>
-        <v>-0.63126663787232851</v>
+        <v>-0.44964746453462529</v>
       </c>
       <c r="C123">
         <f t="shared" si="4"/>
-        <v>0.77556587851024394</v>
+        <v>0.89320611150931051</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
         <f t="shared" si="5"/>
-        <v>5.6999999999999904</v>
+        <v>12.199999999999973</v>
       </c>
       <c r="B124">
         <f t="shared" si="3"/>
-        <v>-0.55068554259764579</v>
+        <v>-0.35822928223685357</v>
       </c>
       <c r="C124">
         <f t="shared" si="4"/>
-        <v>0.83471278483915445</v>
+        <v>0.93363364407462779</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125">
         <f t="shared" si="5"/>
-        <v>5.7999999999999901</v>
+        <v>12.299999999999972</v>
       </c>
       <c r="B125">
         <f t="shared" si="3"/>
-        <v>-0.46460217941376603</v>
+        <v>-0.26323179136582836</v>
       </c>
       <c r="C125">
         <f t="shared" si="4"/>
-        <v>0.88551951694131437</v>
+        <v>0.96473261788660225</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
         <f t="shared" si="5"/>
-        <v>5.8999999999999897</v>
+        <v>12.399999999999972</v>
       </c>
       <c r="B126">
         <f t="shared" si="3"/>
-        <v>-0.3738766648302459</v>
+        <v>-0.16560417544833742</v>
       </c>
       <c r="C126">
         <f t="shared" si="4"/>
-        <v>0.92747843074403191</v>
+        <v>0.9861923022788589</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
         <f t="shared" si="5"/>
-        <v>5.9999999999999893</v>
+        <v>12.499999999999972</v>
       </c>
       <c r="B127">
         <f t="shared" si="3"/>
-        <v>-0.27941549819893613</v>
+        <v>-6.632189735122905E-2</v>
       </c>
       <c r="C127">
         <f t="shared" si="4"/>
-        <v>0.96017028665036308</v>
+        <v>0.99779827917857877</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128">
         <f t="shared" si="5"/>
-        <v>6.099999999999989</v>
+        <v>12.599999999999971</v>
       </c>
       <c r="B128">
         <f t="shared" si="3"/>
-        <v>-0.18216250427210637</v>
+        <v>3.3623047221108288E-2</v>
       </c>
       <c r="C128">
         <f t="shared" si="4"/>
-        <v>0.9832684384425826</v>
+        <v>0.99943458550100572</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129">
         <f t="shared" si="5"/>
-        <v>6.1999999999999886</v>
+        <v>12.699999999999971</v>
       </c>
       <c r="B129">
         <f t="shared" si="3"/>
-        <v>-8.3089402817507901E-2</v>
+        <v>0.13323204141991404</v>
       </c>
       <c r="C129">
         <f t="shared" si="4"/>
-        <v>0.9965420970232165</v>
+        <v>0.99108487181425708</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130">
         <f t="shared" si="5"/>
-        <v>6.2999999999999883</v>
+        <v>12.799999999999971</v>
       </c>
       <c r="B130">
         <f t="shared" si="3"/>
-        <v>1.6813900484338166E-2</v>
+        <v>0.23150982510150958</v>
       </c>
       <c r="C130">
         <f t="shared" si="4"/>
-        <v>0.99985863638341532</v>
+        <v>0.97283256569744236</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131">
         <f t="shared" si="5"/>
-        <v>6.3999999999999879</v>
+        <v>12.89999999999997</v>
       </c>
       <c r="B131">
         <f t="shared" ref="B131:B153" si="6">SIN(A131)</f>
-        <v>0.11654920485048129</v>
+        <v>0.3274744391376645</v>
       </c>
       <c r="C131">
         <f t="shared" ref="C131:C153" si="7">COS(A131)</f>
-        <v>0.99318491875819404</v>
+        <v>0.94486003815987052</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132">
         <f t="shared" ref="A132:A153" si="8">A131+0.1</f>
-        <v>6.4999999999999876</v>
+        <v>12.99999999999997</v>
       </c>
       <c r="B132">
         <f t="shared" si="6"/>
-        <v>0.21511998808780339</v>
+        <v>0.42016703682661349</v>
       </c>
       <c r="C132">
         <f t="shared" si="7"/>
-        <v>0.97658762572802615</v>
+        <v>0.90744678145020885</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133">
         <f t="shared" si="8"/>
-        <v>6.5999999999999872</v>
+        <v>13.099999999999969</v>
       </c>
       <c r="B133">
         <f t="shared" si="6"/>
-        <v>0.31154136351336603</v>
+        <v>0.50866146437234772</v>
       </c>
       <c r="C133">
         <f t="shared" si="7"/>
-        <v>0.95023259195853349</v>
+        <v>0.86096661646232187</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134">
         <f t="shared" si="8"/>
-        <v>6.6999999999999869</v>
+        <v>13.199999999999969</v>
       </c>
       <c r="B134">
         <f t="shared" si="6"/>
-        <v>0.40484992061658615</v>
+        <v>0.59207351470719871</v>
       </c>
       <c r="C134">
         <f t="shared" si="7"/>
-        <v>0.91438314823532474</v>
+        <v>0.80588395764046861</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135">
         <f t="shared" si="8"/>
-        <v>6.7999999999999865</v>
+        <v>13.299999999999969</v>
       </c>
       <c r="B135">
         <f t="shared" si="6"/>
-        <v>0.49411335113859661</v>
+        <v>0.6695697621965786</v>
       </c>
       <c r="C135">
         <f t="shared" si="7"/>
-        <v>0.86939749034983183</v>
+        <v>0.7427491727036909</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136">
         <f t="shared" si="8"/>
-        <v>6.8999999999999861</v>
+        <v>13.399999999999968</v>
       </c>
       <c r="B136">
         <f t="shared" si="6"/>
-        <v>0.57843976438818856</v>
+        <v>0.74037588995242709</v>
       </c>
       <c r="C136">
         <f t="shared" si="7"/>
-        <v>0.81572510012536503</v>
+        <v>0.67219308355349172</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137">
         <f t="shared" si="8"/>
-        <v>6.9999999999999858</v>
+        <v>13.499999999999968</v>
       </c>
       <c r="B137">
         <f t="shared" si="6"/>
-        <v>0.6569865987187784</v>
+        <v>0.80378442655160187</v>
       </c>
       <c r="C137">
         <f t="shared" si="7"/>
-        <v>0.75390225434331393</v>
+        <v>0.59492066330991777</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138">
         <f t="shared" si="8"/>
-        <v>7.0999999999999854</v>
+        <v>13.599999999999968</v>
       </c>
       <c r="B138">
         <f t="shared" si="6"/>
-        <v>0.72896904012586616</v>
+        <v>0.85916181485647947</v>
       </c>
       <c r="C138">
         <f t="shared" si="7"/>
-        <v>0.68454666644281692</v>
+        <v>0.51170399245317644</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139">
         <f t="shared" si="8"/>
-        <v>7.1999999999999851</v>
+        <v>13.699999999999967</v>
       </c>
       <c r="B139">
         <f t="shared" si="6"/>
-        <v>0.79366786384914401</v>
+        <v>0.9059547423084483</v>
       </c>
       <c r="C139">
         <f t="shared" si="7"/>
-        <v>0.60835131453226654</v>
+        <v>0.42337454445069445</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140">
         <f t="shared" si="8"/>
-        <v>7.2999999999999847</v>
+        <v>13.799999999999967</v>
       </c>
       <c r="B140">
         <f t="shared" si="6"/>
-        <v>0.85043662062855652</v>
+        <v>0.94369566944409367</v>
       </c>
       <c r="C140">
         <f t="shared" si="7"/>
-        <v>0.52607751738111819</v>
+        <v>0.33081487794907882</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
         <f t="shared" si="8"/>
-        <v>7.3999999999999844</v>
+        <v>13.899999999999967</v>
       </c>
       <c r="B141">
         <f t="shared" si="6"/>
-        <v>0.89870809581161992</v>
+        <v>0.97200750139496805</v>
       </c>
       <c r="C141">
         <f t="shared" si="7"/>
-        <v>0.43854732757440468</v>
+        <v>0.23494981853985589</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
         <f t="shared" si="8"/>
-        <v>7.499999999999984</v>
+        <v>13.999999999999966</v>
       </c>
       <c r="B142">
         <f t="shared" si="6"/>
-        <v>0.93799997677473335</v>
+        <v>0.99060735569486569</v>
       </c>
       <c r="C142">
         <f t="shared" si="7"/>
-        <v>0.34663531783504081</v>
+        <v>0.13673721820786702</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143">
         <f t="shared" si="8"/>
-        <v>7.5999999999999837</v>
+        <v>14.099999999999966</v>
       </c>
       <c r="B143">
         <f t="shared" si="6"/>
-        <v>0.96791967203148233</v>
+        <v>0.99930938874791642</v>
       </c>
       <c r="C143">
         <f t="shared" si="7"/>
-        <v>0.25125984258227119</v>
+        <v>3.715838479086013E-2</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144">
         <f t="shared" si="8"/>
-        <v>7.6999999999999833</v>
+        <v>14.199999999999966</v>
       </c>
       <c r="B144">
         <f t="shared" si="6"/>
-        <v>0.98816823387699781</v>
+        <v>0.99802665271636382</v>
       </c>
       <c r="C144">
         <f t="shared" si="7"/>
-        <v>0.15337386203788103</v>
+        <v>-6.2791722924048082E-2</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145">
         <f t="shared" si="8"/>
-        <v>7.7999999999999829</v>
+        <v>14.299999999999965</v>
       </c>
       <c r="B145">
         <f t="shared" si="6"/>
-        <v>0.9985433453746041</v>
+        <v>0.98677196427461911</v>
       </c>
       <c r="C145">
         <f t="shared" si="7"/>
-        <v>5.3955420562666605E-2</v>
+        <v>-0.16211443649968321</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146">
         <f t="shared" si="8"/>
-        <v>7.8999999999999826</v>
+        <v>14.399999999999965</v>
       </c>
       <c r="B146">
         <f t="shared" si="6"/>
-        <v>0.99894134183977279</v>
+        <v>0.96565777654928675</v>
       </c>
       <c r="C146">
         <f t="shared" si="7"/>
-        <v>-4.6002125639519206E-2</v>
+        <v>-0.25981735621372154</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147">
         <f t="shared" si="8"/>
-        <v>7.9999999999999822</v>
+        <v>14.499999999999964</v>
       </c>
       <c r="B147">
         <f t="shared" si="6"/>
-        <v>0.98935824662338434</v>
+        <v>0.93489505552469565</v>
       </c>
       <c r="C147">
         <f t="shared" si="7"/>
-        <v>-0.14550003380859594</v>
+        <v>-0.35492426678867178</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148">
         <f t="shared" si="8"/>
-        <v>8.0999999999999819</v>
+        <v>14.599999999999964</v>
       </c>
       <c r="B148">
         <f t="shared" si="6"/>
-        <v>0.96988981084509063</v>
+        <v>0.89479117214052006</v>
       </c>
       <c r="C148">
         <f t="shared" si="7"/>
-        <v>-0.2435441537357739</v>
+        <v>-0.44648489141223385</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149">
         <f t="shared" si="8"/>
-        <v>8.1999999999999815</v>
+        <v>14.699999999999964</v>
       </c>
       <c r="B149">
         <f t="shared" si="6"/>
-        <v>0.94073055667977912</v>
+        <v>0.84574683114295324</v>
       </c>
       <c r="C149">
         <f t="shared" si="7"/>
-        <v>-0.33915486098381781</v>
+        <v>-0.53358438658908769</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150">
         <f t="shared" si="8"/>
-        <v>8.2999999999999812</v>
+        <v>14.799999999999963</v>
       </c>
       <c r="B150">
         <f t="shared" si="6"/>
-        <v>0.90217183375630172</v>
+        <v>0.78825206737533915</v>
       </c>
       <c r="C150">
         <f t="shared" si="7"/>
-        <v>-0.43137684497060319</v>
+        <v>-0.61535248295469136</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151">
         <f t="shared" si="8"/>
-        <v>8.3999999999999808</v>
+        <v>14.899999999999963</v>
       </c>
       <c r="B151">
         <f t="shared" si="6"/>
-        <v>0.85459890808829064</v>
+        <v>0.72288134951200178</v>
       </c>
       <c r="C151">
         <f t="shared" si="7"/>
-        <v>-0.51928865411666891</v>
+        <v>-0.69097218071909894</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152">
         <f t="shared" si="8"/>
-        <v>8.4999999999999805</v>
+        <v>14.999999999999963</v>
       </c>
       <c r="B152">
         <f t="shared" si="6"/>
-        <v>0.79848711262350203</v>
+        <v>0.65028784015714525</v>
       </c>
       <c r="C152">
         <f t="shared" si="7"/>
-        <v>-0.60201190268480798</v>
+        <v>-0.759687912858797</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153">
         <f t="shared" si="8"/>
-        <v>8.5999999999999801</v>
+        <v>15.099999999999962</v>
       </c>
       <c r="B153">
         <f t="shared" si="6"/>
-        <v>0.73439709787412666</v>
+        <v>0.57119686966001926</v>
       </c>
       <c r="C153">
         <f t="shared" si="7"/>
-        <v>-0.67872004731999813</v>
+        <v>-0.82081309449264694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>